<commit_message>
ozon fix 30.09 part 2
</commit_message>
<xml_diff>
--- a/cs.xlsx
+++ b/cs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27F8DD0-4CBD-1643-881C-AC33BEB0EAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DA52CB-4DD6-354E-BDA5-AB4B3B771B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26700" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3198" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3200" uniqueCount="4">
   <si>
     <t>id</t>
   </si>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3197"/>
+  <dimension ref="A1:D3199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3185" zoomScale="67" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E3197" sqref="E3197"/>
+    <sheetView tabSelected="1" topLeftCell="A3177" zoomScale="67" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3200" sqref="A3200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26016,6 +26016,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3198" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3198">
+        <v>4226646</v>
+      </c>
+      <c r="B3198" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3199" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3199">
+        <v>4226635</v>
+      </c>
+      <c r="B3199" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
ozon fix 30.09 part 4
</commit_message>
<xml_diff>
--- a/cs.xlsx
+++ b/cs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DA52CB-4DD6-354E-BDA5-AB4B3B771B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B47952-8483-FC4C-9994-37BAA9257A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26700" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:D3199"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3177" zoomScale="67" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3200" sqref="A3200"/>
+      <selection activeCell="A3198" sqref="A3198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
ozon fixes 16.09.2025 part 3
</commit_message>
<xml_diff>
--- a/cs.xlsx
+++ b/cs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B2AD76-E580-7D42-889F-5E9D871826BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E30701E-217C-F244-A56A-EB3C0F1636AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30920" windowHeight="19700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3204" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3219" uniqueCount="4">
   <si>
     <t>id</t>
   </si>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3203"/>
+  <dimension ref="A1:D3218"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3189" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="E3197" sqref="E3197"/>
+      <selection activeCell="B3224" sqref="B3224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26072,6 +26072,126 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3204" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3204">
+        <v>4107268</v>
+      </c>
+      <c r="B3204" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3205" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3205">
+        <v>4303051</v>
+      </c>
+      <c r="B3205" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3206" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3206">
+        <v>4303055</v>
+      </c>
+      <c r="B3206" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3207" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3207">
+        <v>4131598</v>
+      </c>
+      <c r="B3207" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3208" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3208">
+        <v>4303157</v>
+      </c>
+      <c r="B3208" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3209" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3209">
+        <v>4303158</v>
+      </c>
+      <c r="B3209" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3210" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3210">
+        <v>4130775</v>
+      </c>
+      <c r="B3210" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3211" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3211">
+        <v>4303164</v>
+      </c>
+      <c r="B3211" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3212" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3212">
+        <v>4303165</v>
+      </c>
+      <c r="B3212" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3213" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3213">
+        <v>4157185</v>
+      </c>
+      <c r="B3213" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3214" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3214">
+        <v>4303170</v>
+      </c>
+      <c r="B3214" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3215" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3215">
+        <v>4303171</v>
+      </c>
+      <c r="B3215" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3216" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3216">
+        <v>4222946</v>
+      </c>
+      <c r="B3216" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3217" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3217">
+        <v>4303181</v>
+      </c>
+      <c r="B3217" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3218" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3218">
+        <v>4303182</v>
+      </c>
+      <c r="B3218" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
ozon fixes 21.10.2025 part 1
</commit_message>
<xml_diff>
--- a/cs.xlsx
+++ b/cs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E30701E-217C-F244-A56A-EB3C0F1636AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991950A3-097D-FB41-B1B7-2A749ECCAEF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30920" windowHeight="19700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="30920" windowHeight="19700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3219" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3222" uniqueCount="4">
   <si>
     <t>id</t>
   </si>
@@ -105,9 +105,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -145,7 +145,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -251,7 +251,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -393,7 +393,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3218"/>
+  <dimension ref="A1:D3221"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3189" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <selection activeCell="B3224" sqref="B3224"/>
+      <selection activeCell="B3235" sqref="B3235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -26192,6 +26192,30 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3219" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3219">
+        <v>1052411</v>
+      </c>
+      <c r="B3219" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3220" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3220">
+        <v>1063949</v>
+      </c>
+      <c r="B3220" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3221" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3221">
+        <v>4331106</v>
+      </c>
+      <c r="B3221" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
ozon fixes 15.01.2026 part 6
</commit_message>
<xml_diff>
--- a/cs.xlsx
+++ b/cs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dastanbaitursynov/Documents/GLOBERCE/oz-fmh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58B2100-B9D4-B545-8A37-A21F8E28C5FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055A7919-435E-2641-8EBC-AFF9A3FF4684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="16800" windowHeight="19840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3365" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3367" uniqueCount="4">
   <si>
     <t>id</t>
   </si>
@@ -404,7 +404,7 @@
   <dimension ref="A1:D3366"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3310" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3365" sqref="A3365:A3366"/>
+      <selection activeCell="E3335" sqref="E3335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27364,10 +27364,16 @@
       <c r="A3365">
         <v>4977349</v>
       </c>
+      <c r="B3365" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3366" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3366">
         <v>4977350</v>
+      </c>
+      <c r="B3366" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>